<commit_message>
level shifter doc updated
</commit_message>
<xml_diff>
--- a/doc/33-voltage-protection-check.xlsx
+++ b/doc/33-voltage-protection-check.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="21555" windowHeight="12120"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="21555" windowHeight="12120" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="circuit-emu" sheetId="1" r:id="rId1"/>
+    <sheet name="level_shift_test01" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>test 1</t>
     <phoneticPr fontId="1"/>
@@ -65,12 +66,68 @@
     <t>de0-cv manual simulation</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>off = cp gpio 1 to 0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>on = cp gpio 0 to 1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>dir</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>rst btn</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>inc btn</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>direction</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>btn</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>sw</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>led</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>gpio 0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>gpio 1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>3.3v</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>5v</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,6 +138,14 @@
     </font>
     <font>
       <sz val="6"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <charset val="128"/>
@@ -104,18 +169,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="標準 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1266,6 +1334,4302 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>238124</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>238124</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="正方形/長方形 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="714374" y="2057400"/>
+          <a:ext cx="10715625" cy="3429000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800"/>
+            <a:t>DE0 board</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1800"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="3" name="グループ化 2"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1666875" y="6000750"/>
+          <a:ext cx="238125" cy="514350"/>
+          <a:chOff x="1666875" y="4286250"/>
+          <a:chExt cx="238125" cy="514350"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="4" name="正方形/長方形 3"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="514350"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="5" name="正方形/長方形 4"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="171450"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="6" name="グループ化 5"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="2143125" y="6000750"/>
+          <a:ext cx="238125" cy="514350"/>
+          <a:chOff x="1666875" y="4286250"/>
+          <a:chExt cx="238125" cy="514350"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="7" name="正方形/長方形 6"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="514350"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8" name="正方形/長方形 7"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="171450"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="9" name="グループ化 8"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="2619375" y="6000750"/>
+          <a:ext cx="238125" cy="514350"/>
+          <a:chOff x="1666875" y="4286250"/>
+          <a:chExt cx="238125" cy="514350"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="10" name="正方形/長方形 9"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="514350"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="11" name="正方形/長方形 10"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="171450"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="12" name="グループ化 11"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="3095625" y="6000750"/>
+          <a:ext cx="238125" cy="514350"/>
+          <a:chOff x="1666875" y="4286250"/>
+          <a:chExt cx="238125" cy="514350"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="13" name="正方形/長方形 12"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="514350"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="14" name="正方形/長方形 13"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="171450"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="15" name="グループ化 14"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="3571875" y="6000750"/>
+          <a:ext cx="238125" cy="514350"/>
+          <a:chOff x="1666875" y="4286250"/>
+          <a:chExt cx="238125" cy="514350"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="16" name="正方形/長方形 15"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="514350"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="17" name="正方形/長方形 16"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="171450"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="18" name="グループ化 17"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="4048125" y="6000750"/>
+          <a:ext cx="238125" cy="514350"/>
+          <a:chOff x="1666875" y="4286250"/>
+          <a:chExt cx="238125" cy="514350"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="19" name="正方形/長方形 18"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="514350"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="20" name="正方形/長方形 19"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="171450"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="21" name="グループ化 20"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="4524375" y="6000750"/>
+          <a:ext cx="238125" cy="514350"/>
+          <a:chOff x="1666875" y="4286250"/>
+          <a:chExt cx="238125" cy="514350"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="22" name="正方形/長方形 21"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="514350"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="23" name="正方形/長方形 22"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="171450"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="24" name="グループ化 23"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="5000625" y="6000750"/>
+          <a:ext cx="238125" cy="514350"/>
+          <a:chOff x="1666875" y="4286250"/>
+          <a:chExt cx="238125" cy="514350"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="25" name="正方形/長方形 24"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="514350"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="26" name="正方形/長方形 25"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="171450"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="27" name="グループ化 26"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="5476875" y="6000750"/>
+          <a:ext cx="238125" cy="514350"/>
+          <a:chOff x="1666875" y="4286250"/>
+          <a:chExt cx="238125" cy="514350"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="28" name="正方形/長方形 27"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="514350"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="29" name="正方形/長方形 28"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="171450"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="30" name="グループ化 29"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="5953125" y="6000750"/>
+          <a:ext cx="238125" cy="514350"/>
+          <a:chOff x="1666875" y="4286250"/>
+          <a:chExt cx="238125" cy="514350"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="31" name="正方形/長方形 30"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="514350"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="32" name="正方形/長方形 31"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="171450"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="正方形/長方形 32"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1666875" y="3771900"/>
+          <a:ext cx="238125" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="34" name="正方形/長方形 33"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2143125" y="3771900"/>
+          <a:ext cx="238125" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name="正方形/長方形 34"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2619375" y="3771900"/>
+          <a:ext cx="238125" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="36" name="正方形/長方形 35"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3095625" y="3771900"/>
+          <a:ext cx="238125" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="37" name="正方形/長方形 36"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3571875" y="3771900"/>
+          <a:ext cx="238125" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name="正方形/長方形 37"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4048125" y="3771900"/>
+          <a:ext cx="238125" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="39" name="正方形/長方形 38"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4524375" y="3771900"/>
+          <a:ext cx="238125" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="正方形/長方形 39"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5000625" y="3771900"/>
+          <a:ext cx="238125" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="41" name="正方形/長方形 40"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5476875" y="3771900"/>
+          <a:ext cx="238125" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="42" name="正方形/長方形 41"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5953125" y="3771900"/>
+          <a:ext cx="238125" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="43" name="正方形/長方形 42"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7381875" y="3771900"/>
+          <a:ext cx="238125" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="44" name="正方形/長方形 43"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7858125" y="3771900"/>
+          <a:ext cx="238125" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="45" name="正方形/長方形 44"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8334375" y="3771900"/>
+          <a:ext cx="238125" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="46" name="正方形/長方形 45"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8810625" y="3771900"/>
+          <a:ext cx="238125" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="47" name="正方形/長方形 46"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9286875" y="3771900"/>
+          <a:ext cx="238125" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="48" name="正方形/長方形 47"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9763125" y="3771900"/>
+          <a:ext cx="238125" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="49" name="正方形/長方形 48"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10239375" y="3771900"/>
+          <a:ext cx="238125" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="50" name="正方形/長方形 49"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10715625" y="3771900"/>
+          <a:ext cx="238125" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="51" name="円/楕円 50"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7381875" y="4457700"/>
+          <a:ext cx="476250" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="52" name="円/楕円 51"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8334375" y="4457700"/>
+          <a:ext cx="476250" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="53" name="円/楕円 52"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9286875" y="4457700"/>
+          <a:ext cx="476250" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="54" name="円/楕円 53"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10239375" y="4457700"/>
+          <a:ext cx="476250" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="55" name="正方形/長方形 54"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2505075" y="3600450"/>
+          <a:ext cx="3810000" cy="514350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1800"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="56" name="正方形/長方形 55"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7258050" y="3600450"/>
+          <a:ext cx="3810000" cy="514350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1800"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>238124</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>238124</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="57" name="正方形/長方形 56"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="714374" y="857250"/>
+          <a:ext cx="10715625" cy="2400300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800"/>
+            <a:t>bread board</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1800"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="67" name="グループ化 66"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="2762250" y="2914650"/>
+          <a:ext cx="3333750" cy="2571750"/>
+          <a:chOff x="2619375" y="2914650"/>
+          <a:chExt cx="3333750" cy="2400300"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="59" name="直線コネクタ 58"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="2619375" y="2914650"/>
+            <a:ext cx="0" cy="2400300"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="3">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="60" name="直線コネクタ 59"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="4048125" y="2914650"/>
+            <a:ext cx="0" cy="2400300"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="3">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="61" name="直線コネクタ 60"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="3095625" y="2914650"/>
+            <a:ext cx="0" cy="2400300"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="3">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="62" name="直線コネクタ 61"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="5000625" y="2914650"/>
+            <a:ext cx="0" cy="2400300"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="3">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="63" name="直線コネクタ 62"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="3571875" y="2914650"/>
+            <a:ext cx="0" cy="2400300"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="3">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="64" name="直線コネクタ 63"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="4524375" y="2914650"/>
+            <a:ext cx="0" cy="2400300"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="3">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="65" name="直線コネクタ 64"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="5476875" y="2914650"/>
+            <a:ext cx="0" cy="2400300"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="3">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="66" name="直線コネクタ 65"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="5953125" y="2914650"/>
+            <a:ext cx="0" cy="2400300"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="3">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="68" name="グループ化 67"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="7524750" y="2914650"/>
+          <a:ext cx="3333750" cy="2571750"/>
+          <a:chOff x="2619375" y="2914650"/>
+          <a:chExt cx="3333750" cy="2400300"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="69" name="直線コネクタ 68"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="2619375" y="2914650"/>
+            <a:ext cx="0" cy="2400300"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="3">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="70" name="直線コネクタ 69"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="4048125" y="2914650"/>
+            <a:ext cx="0" cy="2400300"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="3">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="71" name="直線コネクタ 70"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="3095625" y="2914650"/>
+            <a:ext cx="0" cy="2400300"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="3">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="72" name="直線コネクタ 71"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="5000625" y="2914650"/>
+            <a:ext cx="0" cy="2400300"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="3">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="73" name="直線コネクタ 72"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="3571875" y="2914650"/>
+            <a:ext cx="0" cy="2400300"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="3">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="74" name="直線コネクタ 73"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="4524375" y="2914650"/>
+            <a:ext cx="0" cy="2400300"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="3">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="75" name="直線コネクタ 74"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="5476875" y="2914650"/>
+            <a:ext cx="0" cy="2400300"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="3">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="76" name="直線コネクタ 75"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="5953125" y="2914650"/>
+            <a:ext cx="0" cy="2400300"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="3">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="77" name="正方形/長方形 76"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2619375" y="1714500"/>
+          <a:ext cx="8334376" cy="1200150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800"/>
+            <a:t>level shifter</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1800"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="88" name="グループ化 87"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="2762250" y="685800"/>
+          <a:ext cx="8096250" cy="1028701"/>
+          <a:chOff x="2619375" y="1885950"/>
+          <a:chExt cx="8096250" cy="1028701"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="80" name="フリーフォーム 79"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2619375" y="1885951"/>
+            <a:ext cx="4781550" cy="1028700"/>
+          </a:xfrm>
+          <a:custGeom>
+            <a:avLst/>
+            <a:gdLst>
+              <a:gd name="connsiteX0" fmla="*/ 804862 w 6372224"/>
+              <a:gd name="connsiteY0" fmla="*/ 996950 h 1054100"/>
+              <a:gd name="connsiteX1" fmla="*/ 795337 w 6372224"/>
+              <a:gd name="connsiteY1" fmla="*/ 158750 h 1054100"/>
+              <a:gd name="connsiteX2" fmla="*/ 5576887 w 6372224"/>
+              <a:gd name="connsiteY2" fmla="*/ 149225 h 1054100"/>
+              <a:gd name="connsiteX3" fmla="*/ 5567362 w 6372224"/>
+              <a:gd name="connsiteY3" fmla="*/ 1054100 h 1054100"/>
+              <a:gd name="connsiteX0" fmla="*/ 402431 w 5769768"/>
+              <a:gd name="connsiteY0" fmla="*/ 995362 h 1052512"/>
+              <a:gd name="connsiteX1" fmla="*/ 1593056 w 5769768"/>
+              <a:gd name="connsiteY1" fmla="*/ 166687 h 1052512"/>
+              <a:gd name="connsiteX2" fmla="*/ 5174456 w 5769768"/>
+              <a:gd name="connsiteY2" fmla="*/ 147637 h 1052512"/>
+              <a:gd name="connsiteX3" fmla="*/ 5164931 w 5769768"/>
+              <a:gd name="connsiteY3" fmla="*/ 1052512 h 1052512"/>
+              <a:gd name="connsiteX0" fmla="*/ 402431 w 5567362"/>
+              <a:gd name="connsiteY0" fmla="*/ 976312 h 1033462"/>
+              <a:gd name="connsiteX1" fmla="*/ 1593056 w 5567362"/>
+              <a:gd name="connsiteY1" fmla="*/ 147637 h 1033462"/>
+              <a:gd name="connsiteX2" fmla="*/ 4212431 w 5567362"/>
+              <a:gd name="connsiteY2" fmla="*/ 147637 h 1033462"/>
+              <a:gd name="connsiteX3" fmla="*/ 5164931 w 5567362"/>
+              <a:gd name="connsiteY3" fmla="*/ 1033462 h 1033462"/>
+              <a:gd name="connsiteX0" fmla="*/ 402431 w 5567362"/>
+              <a:gd name="connsiteY0" fmla="*/ 971550 h 1000125"/>
+              <a:gd name="connsiteX1" fmla="*/ 1593056 w 5567362"/>
+              <a:gd name="connsiteY1" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX2" fmla="*/ 4212431 w 5567362"/>
+              <a:gd name="connsiteY2" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX3" fmla="*/ 5164931 w 5567362"/>
+              <a:gd name="connsiteY3" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX0" fmla="*/ 402431 w 5567362"/>
+              <a:gd name="connsiteY0" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX1" fmla="*/ 1593056 w 5567362"/>
+              <a:gd name="connsiteY1" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX2" fmla="*/ 4212431 w 5567362"/>
+              <a:gd name="connsiteY2" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX3" fmla="*/ 5164931 w 5567362"/>
+              <a:gd name="connsiteY3" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX0" fmla="*/ 0 w 5164931"/>
+              <a:gd name="connsiteY0" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX1" fmla="*/ 1190625 w 5164931"/>
+              <a:gd name="connsiteY1" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX2" fmla="*/ 3810000 w 5164931"/>
+              <a:gd name="connsiteY2" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX3" fmla="*/ 4762500 w 5164931"/>
+              <a:gd name="connsiteY3" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX0" fmla="*/ 0 w 4781550"/>
+              <a:gd name="connsiteY0" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX1" fmla="*/ 1190625 w 4781550"/>
+              <a:gd name="connsiteY1" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX2" fmla="*/ 3810000 w 4781550"/>
+              <a:gd name="connsiteY2" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX3" fmla="*/ 4762500 w 4781550"/>
+              <a:gd name="connsiteY3" fmla="*/ 1000125 h 1000125"/>
+            </a:gdLst>
+            <a:ahLst/>
+            <a:cxnLst>
+              <a:cxn ang="0">
+                <a:pos x="connsiteX0" y="connsiteY0"/>
+              </a:cxn>
+              <a:cxn ang="0">
+                <a:pos x="connsiteX1" y="connsiteY1"/>
+              </a:cxn>
+              <a:cxn ang="0">
+                <a:pos x="connsiteX2" y="connsiteY2"/>
+              </a:cxn>
+              <a:cxn ang="0">
+                <a:pos x="connsiteX3" y="connsiteY3"/>
+              </a:cxn>
+            </a:cxnLst>
+            <a:rect l="l" t="t" r="r" b="b"/>
+            <a:pathLst>
+              <a:path w="4781550" h="1000125">
+                <a:moveTo>
+                  <a:pt x="0" y="1000125"/>
+                </a:moveTo>
+                <a:cubicBezTo>
+                  <a:pt x="19050" y="346868"/>
+                  <a:pt x="555625" y="285750"/>
+                  <a:pt x="1190625" y="142875"/>
+                </a:cubicBezTo>
+                <a:cubicBezTo>
+                  <a:pt x="1825625" y="0"/>
+                  <a:pt x="3214687" y="0"/>
+                  <a:pt x="3810000" y="142875"/>
+                </a:cubicBezTo>
+                <a:cubicBezTo>
+                  <a:pt x="4405313" y="285750"/>
+                  <a:pt x="4781550" y="488950"/>
+                  <a:pt x="4762500" y="1000125"/>
+                </a:cubicBezTo>
+              </a:path>
+            </a:pathLst>
+          </a:custGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="3">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="81" name="フリーフォーム 80"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3095625" y="1885950"/>
+            <a:ext cx="4781550" cy="1028700"/>
+          </a:xfrm>
+          <a:custGeom>
+            <a:avLst/>
+            <a:gdLst>
+              <a:gd name="connsiteX0" fmla="*/ 804862 w 6372224"/>
+              <a:gd name="connsiteY0" fmla="*/ 996950 h 1054100"/>
+              <a:gd name="connsiteX1" fmla="*/ 795337 w 6372224"/>
+              <a:gd name="connsiteY1" fmla="*/ 158750 h 1054100"/>
+              <a:gd name="connsiteX2" fmla="*/ 5576887 w 6372224"/>
+              <a:gd name="connsiteY2" fmla="*/ 149225 h 1054100"/>
+              <a:gd name="connsiteX3" fmla="*/ 5567362 w 6372224"/>
+              <a:gd name="connsiteY3" fmla="*/ 1054100 h 1054100"/>
+              <a:gd name="connsiteX0" fmla="*/ 402431 w 5769768"/>
+              <a:gd name="connsiteY0" fmla="*/ 995362 h 1052512"/>
+              <a:gd name="connsiteX1" fmla="*/ 1593056 w 5769768"/>
+              <a:gd name="connsiteY1" fmla="*/ 166687 h 1052512"/>
+              <a:gd name="connsiteX2" fmla="*/ 5174456 w 5769768"/>
+              <a:gd name="connsiteY2" fmla="*/ 147637 h 1052512"/>
+              <a:gd name="connsiteX3" fmla="*/ 5164931 w 5769768"/>
+              <a:gd name="connsiteY3" fmla="*/ 1052512 h 1052512"/>
+              <a:gd name="connsiteX0" fmla="*/ 402431 w 5567362"/>
+              <a:gd name="connsiteY0" fmla="*/ 976312 h 1033462"/>
+              <a:gd name="connsiteX1" fmla="*/ 1593056 w 5567362"/>
+              <a:gd name="connsiteY1" fmla="*/ 147637 h 1033462"/>
+              <a:gd name="connsiteX2" fmla="*/ 4212431 w 5567362"/>
+              <a:gd name="connsiteY2" fmla="*/ 147637 h 1033462"/>
+              <a:gd name="connsiteX3" fmla="*/ 5164931 w 5567362"/>
+              <a:gd name="connsiteY3" fmla="*/ 1033462 h 1033462"/>
+              <a:gd name="connsiteX0" fmla="*/ 402431 w 5567362"/>
+              <a:gd name="connsiteY0" fmla="*/ 971550 h 1000125"/>
+              <a:gd name="connsiteX1" fmla="*/ 1593056 w 5567362"/>
+              <a:gd name="connsiteY1" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX2" fmla="*/ 4212431 w 5567362"/>
+              <a:gd name="connsiteY2" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX3" fmla="*/ 5164931 w 5567362"/>
+              <a:gd name="connsiteY3" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX0" fmla="*/ 402431 w 5567362"/>
+              <a:gd name="connsiteY0" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX1" fmla="*/ 1593056 w 5567362"/>
+              <a:gd name="connsiteY1" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX2" fmla="*/ 4212431 w 5567362"/>
+              <a:gd name="connsiteY2" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX3" fmla="*/ 5164931 w 5567362"/>
+              <a:gd name="connsiteY3" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX0" fmla="*/ 0 w 5164931"/>
+              <a:gd name="connsiteY0" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX1" fmla="*/ 1190625 w 5164931"/>
+              <a:gd name="connsiteY1" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX2" fmla="*/ 3810000 w 5164931"/>
+              <a:gd name="connsiteY2" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX3" fmla="*/ 4762500 w 5164931"/>
+              <a:gd name="connsiteY3" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX0" fmla="*/ 0 w 4781550"/>
+              <a:gd name="connsiteY0" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX1" fmla="*/ 1190625 w 4781550"/>
+              <a:gd name="connsiteY1" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX2" fmla="*/ 3810000 w 4781550"/>
+              <a:gd name="connsiteY2" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX3" fmla="*/ 4762500 w 4781550"/>
+              <a:gd name="connsiteY3" fmla="*/ 1000125 h 1000125"/>
+            </a:gdLst>
+            <a:ahLst/>
+            <a:cxnLst>
+              <a:cxn ang="0">
+                <a:pos x="connsiteX0" y="connsiteY0"/>
+              </a:cxn>
+              <a:cxn ang="0">
+                <a:pos x="connsiteX1" y="connsiteY1"/>
+              </a:cxn>
+              <a:cxn ang="0">
+                <a:pos x="connsiteX2" y="connsiteY2"/>
+              </a:cxn>
+              <a:cxn ang="0">
+                <a:pos x="connsiteX3" y="connsiteY3"/>
+              </a:cxn>
+            </a:cxnLst>
+            <a:rect l="l" t="t" r="r" b="b"/>
+            <a:pathLst>
+              <a:path w="4781550" h="1000125">
+                <a:moveTo>
+                  <a:pt x="0" y="1000125"/>
+                </a:moveTo>
+                <a:cubicBezTo>
+                  <a:pt x="19050" y="346868"/>
+                  <a:pt x="555625" y="285750"/>
+                  <a:pt x="1190625" y="142875"/>
+                </a:cubicBezTo>
+                <a:cubicBezTo>
+                  <a:pt x="1825625" y="0"/>
+                  <a:pt x="3214687" y="0"/>
+                  <a:pt x="3810000" y="142875"/>
+                </a:cubicBezTo>
+                <a:cubicBezTo>
+                  <a:pt x="4405313" y="285750"/>
+                  <a:pt x="4781550" y="488950"/>
+                  <a:pt x="4762500" y="1000125"/>
+                </a:cubicBezTo>
+              </a:path>
+            </a:pathLst>
+          </a:custGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="3">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="82" name="フリーフォーム 81"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3552825" y="1885950"/>
+            <a:ext cx="4781550" cy="1028700"/>
+          </a:xfrm>
+          <a:custGeom>
+            <a:avLst/>
+            <a:gdLst>
+              <a:gd name="connsiteX0" fmla="*/ 804862 w 6372224"/>
+              <a:gd name="connsiteY0" fmla="*/ 996950 h 1054100"/>
+              <a:gd name="connsiteX1" fmla="*/ 795337 w 6372224"/>
+              <a:gd name="connsiteY1" fmla="*/ 158750 h 1054100"/>
+              <a:gd name="connsiteX2" fmla="*/ 5576887 w 6372224"/>
+              <a:gd name="connsiteY2" fmla="*/ 149225 h 1054100"/>
+              <a:gd name="connsiteX3" fmla="*/ 5567362 w 6372224"/>
+              <a:gd name="connsiteY3" fmla="*/ 1054100 h 1054100"/>
+              <a:gd name="connsiteX0" fmla="*/ 402431 w 5769768"/>
+              <a:gd name="connsiteY0" fmla="*/ 995362 h 1052512"/>
+              <a:gd name="connsiteX1" fmla="*/ 1593056 w 5769768"/>
+              <a:gd name="connsiteY1" fmla="*/ 166687 h 1052512"/>
+              <a:gd name="connsiteX2" fmla="*/ 5174456 w 5769768"/>
+              <a:gd name="connsiteY2" fmla="*/ 147637 h 1052512"/>
+              <a:gd name="connsiteX3" fmla="*/ 5164931 w 5769768"/>
+              <a:gd name="connsiteY3" fmla="*/ 1052512 h 1052512"/>
+              <a:gd name="connsiteX0" fmla="*/ 402431 w 5567362"/>
+              <a:gd name="connsiteY0" fmla="*/ 976312 h 1033462"/>
+              <a:gd name="connsiteX1" fmla="*/ 1593056 w 5567362"/>
+              <a:gd name="connsiteY1" fmla="*/ 147637 h 1033462"/>
+              <a:gd name="connsiteX2" fmla="*/ 4212431 w 5567362"/>
+              <a:gd name="connsiteY2" fmla="*/ 147637 h 1033462"/>
+              <a:gd name="connsiteX3" fmla="*/ 5164931 w 5567362"/>
+              <a:gd name="connsiteY3" fmla="*/ 1033462 h 1033462"/>
+              <a:gd name="connsiteX0" fmla="*/ 402431 w 5567362"/>
+              <a:gd name="connsiteY0" fmla="*/ 971550 h 1000125"/>
+              <a:gd name="connsiteX1" fmla="*/ 1593056 w 5567362"/>
+              <a:gd name="connsiteY1" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX2" fmla="*/ 4212431 w 5567362"/>
+              <a:gd name="connsiteY2" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX3" fmla="*/ 5164931 w 5567362"/>
+              <a:gd name="connsiteY3" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX0" fmla="*/ 402431 w 5567362"/>
+              <a:gd name="connsiteY0" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX1" fmla="*/ 1593056 w 5567362"/>
+              <a:gd name="connsiteY1" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX2" fmla="*/ 4212431 w 5567362"/>
+              <a:gd name="connsiteY2" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX3" fmla="*/ 5164931 w 5567362"/>
+              <a:gd name="connsiteY3" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX0" fmla="*/ 0 w 5164931"/>
+              <a:gd name="connsiteY0" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX1" fmla="*/ 1190625 w 5164931"/>
+              <a:gd name="connsiteY1" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX2" fmla="*/ 3810000 w 5164931"/>
+              <a:gd name="connsiteY2" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX3" fmla="*/ 4762500 w 5164931"/>
+              <a:gd name="connsiteY3" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX0" fmla="*/ 0 w 4781550"/>
+              <a:gd name="connsiteY0" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX1" fmla="*/ 1190625 w 4781550"/>
+              <a:gd name="connsiteY1" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX2" fmla="*/ 3810000 w 4781550"/>
+              <a:gd name="connsiteY2" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX3" fmla="*/ 4762500 w 4781550"/>
+              <a:gd name="connsiteY3" fmla="*/ 1000125 h 1000125"/>
+            </a:gdLst>
+            <a:ahLst/>
+            <a:cxnLst>
+              <a:cxn ang="0">
+                <a:pos x="connsiteX0" y="connsiteY0"/>
+              </a:cxn>
+              <a:cxn ang="0">
+                <a:pos x="connsiteX1" y="connsiteY1"/>
+              </a:cxn>
+              <a:cxn ang="0">
+                <a:pos x="connsiteX2" y="connsiteY2"/>
+              </a:cxn>
+              <a:cxn ang="0">
+                <a:pos x="connsiteX3" y="connsiteY3"/>
+              </a:cxn>
+            </a:cxnLst>
+            <a:rect l="l" t="t" r="r" b="b"/>
+            <a:pathLst>
+              <a:path w="4781550" h="1000125">
+                <a:moveTo>
+                  <a:pt x="0" y="1000125"/>
+                </a:moveTo>
+                <a:cubicBezTo>
+                  <a:pt x="19050" y="346868"/>
+                  <a:pt x="555625" y="285750"/>
+                  <a:pt x="1190625" y="142875"/>
+                </a:cubicBezTo>
+                <a:cubicBezTo>
+                  <a:pt x="1825625" y="0"/>
+                  <a:pt x="3214687" y="0"/>
+                  <a:pt x="3810000" y="142875"/>
+                </a:cubicBezTo>
+                <a:cubicBezTo>
+                  <a:pt x="4405313" y="285750"/>
+                  <a:pt x="4781550" y="488950"/>
+                  <a:pt x="4762500" y="1000125"/>
+                </a:cubicBezTo>
+              </a:path>
+            </a:pathLst>
+          </a:custGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="3">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="83" name="フリーフォーム 82"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4029075" y="1885950"/>
+            <a:ext cx="4781550" cy="1028700"/>
+          </a:xfrm>
+          <a:custGeom>
+            <a:avLst/>
+            <a:gdLst>
+              <a:gd name="connsiteX0" fmla="*/ 804862 w 6372224"/>
+              <a:gd name="connsiteY0" fmla="*/ 996950 h 1054100"/>
+              <a:gd name="connsiteX1" fmla="*/ 795337 w 6372224"/>
+              <a:gd name="connsiteY1" fmla="*/ 158750 h 1054100"/>
+              <a:gd name="connsiteX2" fmla="*/ 5576887 w 6372224"/>
+              <a:gd name="connsiteY2" fmla="*/ 149225 h 1054100"/>
+              <a:gd name="connsiteX3" fmla="*/ 5567362 w 6372224"/>
+              <a:gd name="connsiteY3" fmla="*/ 1054100 h 1054100"/>
+              <a:gd name="connsiteX0" fmla="*/ 402431 w 5769768"/>
+              <a:gd name="connsiteY0" fmla="*/ 995362 h 1052512"/>
+              <a:gd name="connsiteX1" fmla="*/ 1593056 w 5769768"/>
+              <a:gd name="connsiteY1" fmla="*/ 166687 h 1052512"/>
+              <a:gd name="connsiteX2" fmla="*/ 5174456 w 5769768"/>
+              <a:gd name="connsiteY2" fmla="*/ 147637 h 1052512"/>
+              <a:gd name="connsiteX3" fmla="*/ 5164931 w 5769768"/>
+              <a:gd name="connsiteY3" fmla="*/ 1052512 h 1052512"/>
+              <a:gd name="connsiteX0" fmla="*/ 402431 w 5567362"/>
+              <a:gd name="connsiteY0" fmla="*/ 976312 h 1033462"/>
+              <a:gd name="connsiteX1" fmla="*/ 1593056 w 5567362"/>
+              <a:gd name="connsiteY1" fmla="*/ 147637 h 1033462"/>
+              <a:gd name="connsiteX2" fmla="*/ 4212431 w 5567362"/>
+              <a:gd name="connsiteY2" fmla="*/ 147637 h 1033462"/>
+              <a:gd name="connsiteX3" fmla="*/ 5164931 w 5567362"/>
+              <a:gd name="connsiteY3" fmla="*/ 1033462 h 1033462"/>
+              <a:gd name="connsiteX0" fmla="*/ 402431 w 5567362"/>
+              <a:gd name="connsiteY0" fmla="*/ 971550 h 1000125"/>
+              <a:gd name="connsiteX1" fmla="*/ 1593056 w 5567362"/>
+              <a:gd name="connsiteY1" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX2" fmla="*/ 4212431 w 5567362"/>
+              <a:gd name="connsiteY2" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX3" fmla="*/ 5164931 w 5567362"/>
+              <a:gd name="connsiteY3" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX0" fmla="*/ 402431 w 5567362"/>
+              <a:gd name="connsiteY0" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX1" fmla="*/ 1593056 w 5567362"/>
+              <a:gd name="connsiteY1" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX2" fmla="*/ 4212431 w 5567362"/>
+              <a:gd name="connsiteY2" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX3" fmla="*/ 5164931 w 5567362"/>
+              <a:gd name="connsiteY3" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX0" fmla="*/ 0 w 5164931"/>
+              <a:gd name="connsiteY0" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX1" fmla="*/ 1190625 w 5164931"/>
+              <a:gd name="connsiteY1" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX2" fmla="*/ 3810000 w 5164931"/>
+              <a:gd name="connsiteY2" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX3" fmla="*/ 4762500 w 5164931"/>
+              <a:gd name="connsiteY3" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX0" fmla="*/ 0 w 4781550"/>
+              <a:gd name="connsiteY0" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX1" fmla="*/ 1190625 w 4781550"/>
+              <a:gd name="connsiteY1" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX2" fmla="*/ 3810000 w 4781550"/>
+              <a:gd name="connsiteY2" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX3" fmla="*/ 4762500 w 4781550"/>
+              <a:gd name="connsiteY3" fmla="*/ 1000125 h 1000125"/>
+            </a:gdLst>
+            <a:ahLst/>
+            <a:cxnLst>
+              <a:cxn ang="0">
+                <a:pos x="connsiteX0" y="connsiteY0"/>
+              </a:cxn>
+              <a:cxn ang="0">
+                <a:pos x="connsiteX1" y="connsiteY1"/>
+              </a:cxn>
+              <a:cxn ang="0">
+                <a:pos x="connsiteX2" y="connsiteY2"/>
+              </a:cxn>
+              <a:cxn ang="0">
+                <a:pos x="connsiteX3" y="connsiteY3"/>
+              </a:cxn>
+            </a:cxnLst>
+            <a:rect l="l" t="t" r="r" b="b"/>
+            <a:pathLst>
+              <a:path w="4781550" h="1000125">
+                <a:moveTo>
+                  <a:pt x="0" y="1000125"/>
+                </a:moveTo>
+                <a:cubicBezTo>
+                  <a:pt x="19050" y="346868"/>
+                  <a:pt x="555625" y="285750"/>
+                  <a:pt x="1190625" y="142875"/>
+                </a:cubicBezTo>
+                <a:cubicBezTo>
+                  <a:pt x="1825625" y="0"/>
+                  <a:pt x="3214687" y="0"/>
+                  <a:pt x="3810000" y="142875"/>
+                </a:cubicBezTo>
+                <a:cubicBezTo>
+                  <a:pt x="4405313" y="285750"/>
+                  <a:pt x="4781550" y="488950"/>
+                  <a:pt x="4762500" y="1000125"/>
+                </a:cubicBezTo>
+              </a:path>
+            </a:pathLst>
+          </a:custGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="3">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="84" name="フリーフォーム 83"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4505325" y="1885950"/>
+            <a:ext cx="4781550" cy="1028700"/>
+          </a:xfrm>
+          <a:custGeom>
+            <a:avLst/>
+            <a:gdLst>
+              <a:gd name="connsiteX0" fmla="*/ 804862 w 6372224"/>
+              <a:gd name="connsiteY0" fmla="*/ 996950 h 1054100"/>
+              <a:gd name="connsiteX1" fmla="*/ 795337 w 6372224"/>
+              <a:gd name="connsiteY1" fmla="*/ 158750 h 1054100"/>
+              <a:gd name="connsiteX2" fmla="*/ 5576887 w 6372224"/>
+              <a:gd name="connsiteY2" fmla="*/ 149225 h 1054100"/>
+              <a:gd name="connsiteX3" fmla="*/ 5567362 w 6372224"/>
+              <a:gd name="connsiteY3" fmla="*/ 1054100 h 1054100"/>
+              <a:gd name="connsiteX0" fmla="*/ 402431 w 5769768"/>
+              <a:gd name="connsiteY0" fmla="*/ 995362 h 1052512"/>
+              <a:gd name="connsiteX1" fmla="*/ 1593056 w 5769768"/>
+              <a:gd name="connsiteY1" fmla="*/ 166687 h 1052512"/>
+              <a:gd name="connsiteX2" fmla="*/ 5174456 w 5769768"/>
+              <a:gd name="connsiteY2" fmla="*/ 147637 h 1052512"/>
+              <a:gd name="connsiteX3" fmla="*/ 5164931 w 5769768"/>
+              <a:gd name="connsiteY3" fmla="*/ 1052512 h 1052512"/>
+              <a:gd name="connsiteX0" fmla="*/ 402431 w 5567362"/>
+              <a:gd name="connsiteY0" fmla="*/ 976312 h 1033462"/>
+              <a:gd name="connsiteX1" fmla="*/ 1593056 w 5567362"/>
+              <a:gd name="connsiteY1" fmla="*/ 147637 h 1033462"/>
+              <a:gd name="connsiteX2" fmla="*/ 4212431 w 5567362"/>
+              <a:gd name="connsiteY2" fmla="*/ 147637 h 1033462"/>
+              <a:gd name="connsiteX3" fmla="*/ 5164931 w 5567362"/>
+              <a:gd name="connsiteY3" fmla="*/ 1033462 h 1033462"/>
+              <a:gd name="connsiteX0" fmla="*/ 402431 w 5567362"/>
+              <a:gd name="connsiteY0" fmla="*/ 971550 h 1000125"/>
+              <a:gd name="connsiteX1" fmla="*/ 1593056 w 5567362"/>
+              <a:gd name="connsiteY1" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX2" fmla="*/ 4212431 w 5567362"/>
+              <a:gd name="connsiteY2" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX3" fmla="*/ 5164931 w 5567362"/>
+              <a:gd name="connsiteY3" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX0" fmla="*/ 402431 w 5567362"/>
+              <a:gd name="connsiteY0" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX1" fmla="*/ 1593056 w 5567362"/>
+              <a:gd name="connsiteY1" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX2" fmla="*/ 4212431 w 5567362"/>
+              <a:gd name="connsiteY2" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX3" fmla="*/ 5164931 w 5567362"/>
+              <a:gd name="connsiteY3" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX0" fmla="*/ 0 w 5164931"/>
+              <a:gd name="connsiteY0" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX1" fmla="*/ 1190625 w 5164931"/>
+              <a:gd name="connsiteY1" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX2" fmla="*/ 3810000 w 5164931"/>
+              <a:gd name="connsiteY2" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX3" fmla="*/ 4762500 w 5164931"/>
+              <a:gd name="connsiteY3" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX0" fmla="*/ 0 w 4781550"/>
+              <a:gd name="connsiteY0" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX1" fmla="*/ 1190625 w 4781550"/>
+              <a:gd name="connsiteY1" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX2" fmla="*/ 3810000 w 4781550"/>
+              <a:gd name="connsiteY2" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX3" fmla="*/ 4762500 w 4781550"/>
+              <a:gd name="connsiteY3" fmla="*/ 1000125 h 1000125"/>
+            </a:gdLst>
+            <a:ahLst/>
+            <a:cxnLst>
+              <a:cxn ang="0">
+                <a:pos x="connsiteX0" y="connsiteY0"/>
+              </a:cxn>
+              <a:cxn ang="0">
+                <a:pos x="connsiteX1" y="connsiteY1"/>
+              </a:cxn>
+              <a:cxn ang="0">
+                <a:pos x="connsiteX2" y="connsiteY2"/>
+              </a:cxn>
+              <a:cxn ang="0">
+                <a:pos x="connsiteX3" y="connsiteY3"/>
+              </a:cxn>
+            </a:cxnLst>
+            <a:rect l="l" t="t" r="r" b="b"/>
+            <a:pathLst>
+              <a:path w="4781550" h="1000125">
+                <a:moveTo>
+                  <a:pt x="0" y="1000125"/>
+                </a:moveTo>
+                <a:cubicBezTo>
+                  <a:pt x="19050" y="346868"/>
+                  <a:pt x="555625" y="285750"/>
+                  <a:pt x="1190625" y="142875"/>
+                </a:cubicBezTo>
+                <a:cubicBezTo>
+                  <a:pt x="1825625" y="0"/>
+                  <a:pt x="3214687" y="0"/>
+                  <a:pt x="3810000" y="142875"/>
+                </a:cubicBezTo>
+                <a:cubicBezTo>
+                  <a:pt x="4405313" y="285750"/>
+                  <a:pt x="4781550" y="488950"/>
+                  <a:pt x="4762500" y="1000125"/>
+                </a:cubicBezTo>
+              </a:path>
+            </a:pathLst>
+          </a:custGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="3">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="85" name="フリーフォーム 84"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4981575" y="1885950"/>
+            <a:ext cx="4781550" cy="1028700"/>
+          </a:xfrm>
+          <a:custGeom>
+            <a:avLst/>
+            <a:gdLst>
+              <a:gd name="connsiteX0" fmla="*/ 804862 w 6372224"/>
+              <a:gd name="connsiteY0" fmla="*/ 996950 h 1054100"/>
+              <a:gd name="connsiteX1" fmla="*/ 795337 w 6372224"/>
+              <a:gd name="connsiteY1" fmla="*/ 158750 h 1054100"/>
+              <a:gd name="connsiteX2" fmla="*/ 5576887 w 6372224"/>
+              <a:gd name="connsiteY2" fmla="*/ 149225 h 1054100"/>
+              <a:gd name="connsiteX3" fmla="*/ 5567362 w 6372224"/>
+              <a:gd name="connsiteY3" fmla="*/ 1054100 h 1054100"/>
+              <a:gd name="connsiteX0" fmla="*/ 402431 w 5769768"/>
+              <a:gd name="connsiteY0" fmla="*/ 995362 h 1052512"/>
+              <a:gd name="connsiteX1" fmla="*/ 1593056 w 5769768"/>
+              <a:gd name="connsiteY1" fmla="*/ 166687 h 1052512"/>
+              <a:gd name="connsiteX2" fmla="*/ 5174456 w 5769768"/>
+              <a:gd name="connsiteY2" fmla="*/ 147637 h 1052512"/>
+              <a:gd name="connsiteX3" fmla="*/ 5164931 w 5769768"/>
+              <a:gd name="connsiteY3" fmla="*/ 1052512 h 1052512"/>
+              <a:gd name="connsiteX0" fmla="*/ 402431 w 5567362"/>
+              <a:gd name="connsiteY0" fmla="*/ 976312 h 1033462"/>
+              <a:gd name="connsiteX1" fmla="*/ 1593056 w 5567362"/>
+              <a:gd name="connsiteY1" fmla="*/ 147637 h 1033462"/>
+              <a:gd name="connsiteX2" fmla="*/ 4212431 w 5567362"/>
+              <a:gd name="connsiteY2" fmla="*/ 147637 h 1033462"/>
+              <a:gd name="connsiteX3" fmla="*/ 5164931 w 5567362"/>
+              <a:gd name="connsiteY3" fmla="*/ 1033462 h 1033462"/>
+              <a:gd name="connsiteX0" fmla="*/ 402431 w 5567362"/>
+              <a:gd name="connsiteY0" fmla="*/ 971550 h 1000125"/>
+              <a:gd name="connsiteX1" fmla="*/ 1593056 w 5567362"/>
+              <a:gd name="connsiteY1" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX2" fmla="*/ 4212431 w 5567362"/>
+              <a:gd name="connsiteY2" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX3" fmla="*/ 5164931 w 5567362"/>
+              <a:gd name="connsiteY3" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX0" fmla="*/ 402431 w 5567362"/>
+              <a:gd name="connsiteY0" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX1" fmla="*/ 1593056 w 5567362"/>
+              <a:gd name="connsiteY1" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX2" fmla="*/ 4212431 w 5567362"/>
+              <a:gd name="connsiteY2" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX3" fmla="*/ 5164931 w 5567362"/>
+              <a:gd name="connsiteY3" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX0" fmla="*/ 0 w 5164931"/>
+              <a:gd name="connsiteY0" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX1" fmla="*/ 1190625 w 5164931"/>
+              <a:gd name="connsiteY1" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX2" fmla="*/ 3810000 w 5164931"/>
+              <a:gd name="connsiteY2" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX3" fmla="*/ 4762500 w 5164931"/>
+              <a:gd name="connsiteY3" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX0" fmla="*/ 0 w 4781550"/>
+              <a:gd name="connsiteY0" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX1" fmla="*/ 1190625 w 4781550"/>
+              <a:gd name="connsiteY1" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX2" fmla="*/ 3810000 w 4781550"/>
+              <a:gd name="connsiteY2" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX3" fmla="*/ 4762500 w 4781550"/>
+              <a:gd name="connsiteY3" fmla="*/ 1000125 h 1000125"/>
+            </a:gdLst>
+            <a:ahLst/>
+            <a:cxnLst>
+              <a:cxn ang="0">
+                <a:pos x="connsiteX0" y="connsiteY0"/>
+              </a:cxn>
+              <a:cxn ang="0">
+                <a:pos x="connsiteX1" y="connsiteY1"/>
+              </a:cxn>
+              <a:cxn ang="0">
+                <a:pos x="connsiteX2" y="connsiteY2"/>
+              </a:cxn>
+              <a:cxn ang="0">
+                <a:pos x="connsiteX3" y="connsiteY3"/>
+              </a:cxn>
+            </a:cxnLst>
+            <a:rect l="l" t="t" r="r" b="b"/>
+            <a:pathLst>
+              <a:path w="4781550" h="1000125">
+                <a:moveTo>
+                  <a:pt x="0" y="1000125"/>
+                </a:moveTo>
+                <a:cubicBezTo>
+                  <a:pt x="19050" y="346868"/>
+                  <a:pt x="555625" y="285750"/>
+                  <a:pt x="1190625" y="142875"/>
+                </a:cubicBezTo>
+                <a:cubicBezTo>
+                  <a:pt x="1825625" y="0"/>
+                  <a:pt x="3214687" y="0"/>
+                  <a:pt x="3810000" y="142875"/>
+                </a:cubicBezTo>
+                <a:cubicBezTo>
+                  <a:pt x="4405313" y="285750"/>
+                  <a:pt x="4781550" y="488950"/>
+                  <a:pt x="4762500" y="1000125"/>
+                </a:cubicBezTo>
+              </a:path>
+            </a:pathLst>
+          </a:custGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="3">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="86" name="フリーフォーム 85"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5457825" y="1885950"/>
+            <a:ext cx="4781550" cy="1028700"/>
+          </a:xfrm>
+          <a:custGeom>
+            <a:avLst/>
+            <a:gdLst>
+              <a:gd name="connsiteX0" fmla="*/ 804862 w 6372224"/>
+              <a:gd name="connsiteY0" fmla="*/ 996950 h 1054100"/>
+              <a:gd name="connsiteX1" fmla="*/ 795337 w 6372224"/>
+              <a:gd name="connsiteY1" fmla="*/ 158750 h 1054100"/>
+              <a:gd name="connsiteX2" fmla="*/ 5576887 w 6372224"/>
+              <a:gd name="connsiteY2" fmla="*/ 149225 h 1054100"/>
+              <a:gd name="connsiteX3" fmla="*/ 5567362 w 6372224"/>
+              <a:gd name="connsiteY3" fmla="*/ 1054100 h 1054100"/>
+              <a:gd name="connsiteX0" fmla="*/ 402431 w 5769768"/>
+              <a:gd name="connsiteY0" fmla="*/ 995362 h 1052512"/>
+              <a:gd name="connsiteX1" fmla="*/ 1593056 w 5769768"/>
+              <a:gd name="connsiteY1" fmla="*/ 166687 h 1052512"/>
+              <a:gd name="connsiteX2" fmla="*/ 5174456 w 5769768"/>
+              <a:gd name="connsiteY2" fmla="*/ 147637 h 1052512"/>
+              <a:gd name="connsiteX3" fmla="*/ 5164931 w 5769768"/>
+              <a:gd name="connsiteY3" fmla="*/ 1052512 h 1052512"/>
+              <a:gd name="connsiteX0" fmla="*/ 402431 w 5567362"/>
+              <a:gd name="connsiteY0" fmla="*/ 976312 h 1033462"/>
+              <a:gd name="connsiteX1" fmla="*/ 1593056 w 5567362"/>
+              <a:gd name="connsiteY1" fmla="*/ 147637 h 1033462"/>
+              <a:gd name="connsiteX2" fmla="*/ 4212431 w 5567362"/>
+              <a:gd name="connsiteY2" fmla="*/ 147637 h 1033462"/>
+              <a:gd name="connsiteX3" fmla="*/ 5164931 w 5567362"/>
+              <a:gd name="connsiteY3" fmla="*/ 1033462 h 1033462"/>
+              <a:gd name="connsiteX0" fmla="*/ 402431 w 5567362"/>
+              <a:gd name="connsiteY0" fmla="*/ 971550 h 1000125"/>
+              <a:gd name="connsiteX1" fmla="*/ 1593056 w 5567362"/>
+              <a:gd name="connsiteY1" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX2" fmla="*/ 4212431 w 5567362"/>
+              <a:gd name="connsiteY2" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX3" fmla="*/ 5164931 w 5567362"/>
+              <a:gd name="connsiteY3" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX0" fmla="*/ 402431 w 5567362"/>
+              <a:gd name="connsiteY0" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX1" fmla="*/ 1593056 w 5567362"/>
+              <a:gd name="connsiteY1" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX2" fmla="*/ 4212431 w 5567362"/>
+              <a:gd name="connsiteY2" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX3" fmla="*/ 5164931 w 5567362"/>
+              <a:gd name="connsiteY3" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX0" fmla="*/ 0 w 5164931"/>
+              <a:gd name="connsiteY0" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX1" fmla="*/ 1190625 w 5164931"/>
+              <a:gd name="connsiteY1" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX2" fmla="*/ 3810000 w 5164931"/>
+              <a:gd name="connsiteY2" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX3" fmla="*/ 4762500 w 5164931"/>
+              <a:gd name="connsiteY3" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX0" fmla="*/ 0 w 4781550"/>
+              <a:gd name="connsiteY0" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX1" fmla="*/ 1190625 w 4781550"/>
+              <a:gd name="connsiteY1" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX2" fmla="*/ 3810000 w 4781550"/>
+              <a:gd name="connsiteY2" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX3" fmla="*/ 4762500 w 4781550"/>
+              <a:gd name="connsiteY3" fmla="*/ 1000125 h 1000125"/>
+            </a:gdLst>
+            <a:ahLst/>
+            <a:cxnLst>
+              <a:cxn ang="0">
+                <a:pos x="connsiteX0" y="connsiteY0"/>
+              </a:cxn>
+              <a:cxn ang="0">
+                <a:pos x="connsiteX1" y="connsiteY1"/>
+              </a:cxn>
+              <a:cxn ang="0">
+                <a:pos x="connsiteX2" y="connsiteY2"/>
+              </a:cxn>
+              <a:cxn ang="0">
+                <a:pos x="connsiteX3" y="connsiteY3"/>
+              </a:cxn>
+            </a:cxnLst>
+            <a:rect l="l" t="t" r="r" b="b"/>
+            <a:pathLst>
+              <a:path w="4781550" h="1000125">
+                <a:moveTo>
+                  <a:pt x="0" y="1000125"/>
+                </a:moveTo>
+                <a:cubicBezTo>
+                  <a:pt x="19050" y="346868"/>
+                  <a:pt x="555625" y="285750"/>
+                  <a:pt x="1190625" y="142875"/>
+                </a:cubicBezTo>
+                <a:cubicBezTo>
+                  <a:pt x="1825625" y="0"/>
+                  <a:pt x="3214687" y="0"/>
+                  <a:pt x="3810000" y="142875"/>
+                </a:cubicBezTo>
+                <a:cubicBezTo>
+                  <a:pt x="4405313" y="285750"/>
+                  <a:pt x="4781550" y="488950"/>
+                  <a:pt x="4762500" y="1000125"/>
+                </a:cubicBezTo>
+              </a:path>
+            </a:pathLst>
+          </a:custGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="3">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="87" name="フリーフォーム 86"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5934075" y="1885950"/>
+            <a:ext cx="4781550" cy="1028700"/>
+          </a:xfrm>
+          <a:custGeom>
+            <a:avLst/>
+            <a:gdLst>
+              <a:gd name="connsiteX0" fmla="*/ 804862 w 6372224"/>
+              <a:gd name="connsiteY0" fmla="*/ 996950 h 1054100"/>
+              <a:gd name="connsiteX1" fmla="*/ 795337 w 6372224"/>
+              <a:gd name="connsiteY1" fmla="*/ 158750 h 1054100"/>
+              <a:gd name="connsiteX2" fmla="*/ 5576887 w 6372224"/>
+              <a:gd name="connsiteY2" fmla="*/ 149225 h 1054100"/>
+              <a:gd name="connsiteX3" fmla="*/ 5567362 w 6372224"/>
+              <a:gd name="connsiteY3" fmla="*/ 1054100 h 1054100"/>
+              <a:gd name="connsiteX0" fmla="*/ 402431 w 5769768"/>
+              <a:gd name="connsiteY0" fmla="*/ 995362 h 1052512"/>
+              <a:gd name="connsiteX1" fmla="*/ 1593056 w 5769768"/>
+              <a:gd name="connsiteY1" fmla="*/ 166687 h 1052512"/>
+              <a:gd name="connsiteX2" fmla="*/ 5174456 w 5769768"/>
+              <a:gd name="connsiteY2" fmla="*/ 147637 h 1052512"/>
+              <a:gd name="connsiteX3" fmla="*/ 5164931 w 5769768"/>
+              <a:gd name="connsiteY3" fmla="*/ 1052512 h 1052512"/>
+              <a:gd name="connsiteX0" fmla="*/ 402431 w 5567362"/>
+              <a:gd name="connsiteY0" fmla="*/ 976312 h 1033462"/>
+              <a:gd name="connsiteX1" fmla="*/ 1593056 w 5567362"/>
+              <a:gd name="connsiteY1" fmla="*/ 147637 h 1033462"/>
+              <a:gd name="connsiteX2" fmla="*/ 4212431 w 5567362"/>
+              <a:gd name="connsiteY2" fmla="*/ 147637 h 1033462"/>
+              <a:gd name="connsiteX3" fmla="*/ 5164931 w 5567362"/>
+              <a:gd name="connsiteY3" fmla="*/ 1033462 h 1033462"/>
+              <a:gd name="connsiteX0" fmla="*/ 402431 w 5567362"/>
+              <a:gd name="connsiteY0" fmla="*/ 971550 h 1000125"/>
+              <a:gd name="connsiteX1" fmla="*/ 1593056 w 5567362"/>
+              <a:gd name="connsiteY1" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX2" fmla="*/ 4212431 w 5567362"/>
+              <a:gd name="connsiteY2" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX3" fmla="*/ 5164931 w 5567362"/>
+              <a:gd name="connsiteY3" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX0" fmla="*/ 402431 w 5567362"/>
+              <a:gd name="connsiteY0" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX1" fmla="*/ 1593056 w 5567362"/>
+              <a:gd name="connsiteY1" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX2" fmla="*/ 4212431 w 5567362"/>
+              <a:gd name="connsiteY2" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX3" fmla="*/ 5164931 w 5567362"/>
+              <a:gd name="connsiteY3" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX0" fmla="*/ 0 w 5164931"/>
+              <a:gd name="connsiteY0" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX1" fmla="*/ 1190625 w 5164931"/>
+              <a:gd name="connsiteY1" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX2" fmla="*/ 3810000 w 5164931"/>
+              <a:gd name="connsiteY2" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX3" fmla="*/ 4762500 w 5164931"/>
+              <a:gd name="connsiteY3" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX0" fmla="*/ 0 w 4781550"/>
+              <a:gd name="connsiteY0" fmla="*/ 1000125 h 1000125"/>
+              <a:gd name="connsiteX1" fmla="*/ 1190625 w 4781550"/>
+              <a:gd name="connsiteY1" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX2" fmla="*/ 3810000 w 4781550"/>
+              <a:gd name="connsiteY2" fmla="*/ 142875 h 1000125"/>
+              <a:gd name="connsiteX3" fmla="*/ 4762500 w 4781550"/>
+              <a:gd name="connsiteY3" fmla="*/ 1000125 h 1000125"/>
+            </a:gdLst>
+            <a:ahLst/>
+            <a:cxnLst>
+              <a:cxn ang="0">
+                <a:pos x="connsiteX0" y="connsiteY0"/>
+              </a:cxn>
+              <a:cxn ang="0">
+                <a:pos x="connsiteX1" y="connsiteY1"/>
+              </a:cxn>
+              <a:cxn ang="0">
+                <a:pos x="connsiteX2" y="connsiteY2"/>
+              </a:cxn>
+              <a:cxn ang="0">
+                <a:pos x="connsiteX3" y="connsiteY3"/>
+              </a:cxn>
+            </a:cxnLst>
+            <a:rect l="l" t="t" r="r" b="b"/>
+            <a:pathLst>
+              <a:path w="4781550" h="1000125">
+                <a:moveTo>
+                  <a:pt x="0" y="1000125"/>
+                </a:moveTo>
+                <a:cubicBezTo>
+                  <a:pt x="19050" y="346868"/>
+                  <a:pt x="555625" y="285750"/>
+                  <a:pt x="1190625" y="142875"/>
+                </a:cubicBezTo>
+                <a:cubicBezTo>
+                  <a:pt x="1825625" y="0"/>
+                  <a:pt x="3214687" y="0"/>
+                  <a:pt x="3810000" y="142875"/>
+                </a:cubicBezTo>
+                <a:cubicBezTo>
+                  <a:pt x="4405313" y="285750"/>
+                  <a:pt x="4781550" y="488950"/>
+                  <a:pt x="4762500" y="1000125"/>
+                </a:cubicBezTo>
+              </a:path>
+            </a:pathLst>
+          </a:custGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="3">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1558,8 +5922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:E213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A273" workbookViewId="0">
-      <selection activeCell="Q288" sqref="Q288"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1649,14 +6013,178 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="F9:AT45"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="BI20" sqref="BI20:BI21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="16384" width="3.125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="9" spans="10:10">
+      <c r="J9" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="10:32">
+      <c r="J18" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="10:32">
+      <c r="L30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF30" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="6:46">
+      <c r="F34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H34" s="1">
+        <v>9</v>
+      </c>
+      <c r="J34" s="1">
+        <v>8</v>
+      </c>
+      <c r="L34" s="1">
+        <v>7</v>
+      </c>
+      <c r="N34" s="1">
+        <v>6</v>
+      </c>
+      <c r="P34" s="1">
+        <v>5</v>
+      </c>
+      <c r="R34" s="1">
+        <v>4</v>
+      </c>
+      <c r="T34" s="1">
+        <v>3</v>
+      </c>
+      <c r="V34" s="1">
+        <v>2</v>
+      </c>
+      <c r="X34" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z34" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF34" s="1">
+        <v>7</v>
+      </c>
+      <c r="AH34" s="1">
+        <v>6</v>
+      </c>
+      <c r="AJ34" s="1">
+        <v>5</v>
+      </c>
+      <c r="AL34" s="1">
+        <v>4</v>
+      </c>
+      <c r="AN34" s="1">
+        <v>3</v>
+      </c>
+      <c r="AP34" s="1">
+        <v>2</v>
+      </c>
+      <c r="AR34" s="1">
+        <v>1</v>
+      </c>
+      <c r="AT34" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="6:46">
+      <c r="F39" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H39" s="1">
+        <v>9</v>
+      </c>
+      <c r="J39" s="1">
+        <v>8</v>
+      </c>
+      <c r="L39" s="1">
+        <v>7</v>
+      </c>
+      <c r="N39" s="1">
+        <v>6</v>
+      </c>
+      <c r="P39" s="1">
+        <v>5</v>
+      </c>
+      <c r="R39" s="1">
+        <v>4</v>
+      </c>
+      <c r="T39" s="1">
+        <v>3</v>
+      </c>
+      <c r="V39" s="1">
+        <v>2</v>
+      </c>
+      <c r="X39" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z39" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD39" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AG39" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK39" s="1">
+        <v>2</v>
+      </c>
+      <c r="AO39" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS39" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="6:46">
+      <c r="H41" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AG41" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AS41" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="6:46">
+      <c r="H44" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="6:46">
+      <c r="H45" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1671,4 +6199,17 @@
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
slow down count up.
</commit_message>
<xml_diff>
--- a/doc/33-voltage-protection-check.xlsx
+++ b/doc/33-voltage-protection-check.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>test 1</t>
     <phoneticPr fontId="1"/>
@@ -120,6 +120,10 @@
   </si>
   <si>
     <t>5v</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>count divide sw</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -6015,8 +6019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="F9:AT45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="BI20" sqref="BI20:BI21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="13.5"/>
@@ -6152,6 +6156,11 @@
       </c>
       <c r="AS39" s="1">
         <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="6:46">
+      <c r="J40" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="41" spans="6:46">

</xml_diff>

<commit_message>
logic analyzer test ok.
</commit_message>
<xml_diff>
--- a/doc/33-voltage-protection-check.xlsx
+++ b/doc/33-voltage-protection-check.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="21555" windowHeight="12120" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="21555" windowHeight="12120" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="circuit-emu" sheetId="1" r:id="rId1"/>
     <sheet name="level_shift_test01" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="logic-analyzer-result" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -5634,6 +5634,189 @@
         </xdr:txBody>
       </xdr:sp>
     </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2049" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect r="2500" b="66667"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="17830800" cy="3429000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="円/楕円 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6477000" y="2228850"/>
+          <a:ext cx="5181600" cy="1371600"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="角丸四角形吹き出し 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9058275" y="4152900"/>
+          <a:ext cx="1914525" cy="819150"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -39738"/>
+            <a:gd name="adj2" fmla="val -138662"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>2 clocks delayed.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>no</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
+            <a:t> difference btn level shifter and diode level change.</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -5926,7 +6109,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:E213"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A80" workbookViewId="0">
       <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
@@ -6019,7 +6202,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="F9:AT45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
@@ -6201,12 +6384,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="Q23" sqref="Q23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>